<commit_message>
Ajout de la heatmaps pour prendre en compte à la fois la surface terrière et le DBH
</commit_message>
<xml_diff>
--- a/modèle bayésien/Modèle bayésien (simulation).xlsx
+++ b/modèle bayésien/Modèle bayésien (simulation).xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maud Otello\Documents\cours_r\Stage_M2\script\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maud Otello\Documents\cours_r\Stage_M2\script\modèle bayésien\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6490"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16485" windowHeight="6490"/>
   </bookViews>
   <sheets>
     <sheet name="Modèle" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="117">
   <si>
     <t>Modèle</t>
   </si>
@@ -421,6 +421,39 @@
   </si>
   <si>
     <t>Everything is OK</t>
+  </si>
+  <si>
+    <t>fit_heatmap</t>
+  </si>
+  <si>
+    <t>Sortir Y_pred qui prend en compte G et DBH pour faire à la suite un heatmap</t>
+  </si>
+  <si>
+    <t>m_heatmap</t>
+  </si>
+  <si>
+    <t>Y = softmax(alpha + beta*X_cr[n] + gamma*(X_cr[n])^2 + delta*Z_cr[n]+ epsilon*(Z_cr[n])^2)</t>
+  </si>
+  <si>
+    <t>8h23,10h43 ordi plante</t>
+  </si>
+  <si>
+    <t>Après avoir fait tourner les chaines il a du mal et s'arrête</t>
+  </si>
+  <si>
+    <t>3h</t>
+  </si>
+  <si>
+    <t>Foireux car seulement 10 itération qui ne permet pas. L'extraction des Y_préd prend vraiment bcp de temps</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sortir Y_pred qui prend en compte G et DBH pour faire à la suite un heatmap (réduction du nombre de Z_pred (0.1) et X_pred (5) calculer </t>
+  </si>
+  <si>
+    <t>ça va beaucoup plus vite. Il converge même si R dit que non moi je trouve que une RHAT de 1.08 c'est bien.</t>
+  </si>
+  <si>
+    <t>6min</t>
   </si>
 </sst>
 </file>
@@ -836,11 +869,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L24"/>
+  <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -1618,6 +1651,120 @@
       </c>
       <c r="L24" s="13" t="s">
         <v>105</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="73.75" x14ac:dyDescent="0.75">
+      <c r="A25" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B25" s="2">
+        <v>3</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="H25" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="I25" s="13">
+        <v>6</v>
+      </c>
+      <c r="J25" s="2">
+        <v>100</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="L25" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="73.75" x14ac:dyDescent="0.75">
+      <c r="A26" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B26" s="2">
+        <v>3</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="H26" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="I26" s="13">
+        <v>6</v>
+      </c>
+      <c r="J26" s="2">
+        <v>10</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="L26" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="73.75" x14ac:dyDescent="0.75">
+      <c r="A27" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B27" s="2">
+        <v>3</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="H27" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="I27" s="13">
+        <v>6</v>
+      </c>
+      <c r="J27" s="2">
+        <v>100</v>
+      </c>
+      <c r="K27" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="L27" s="2" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>